<commit_message>
Update Manual Tagging of Locations.xlsx
</commit_message>
<xml_diff>
--- a/data/Manual Tagging of Locations.xlsx
+++ b/data/Manual Tagging of Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MadwolfDT\ISSS608_G1_T08\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE11A5-D5DA-4F13-A77D-EEA07B268366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E453F-97BC-4255-8ABC-AEDB66483A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C2011E7-F6C6-464F-B867-BA705ABE8868}"/>
   </bookViews>
@@ -624,13 +624,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB98B35C-41A4-4B67-8D87-B234B1CA3FCD}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="M92" sqref="M92"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="Q101" sqref="Q101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.42578125" style="3" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>